<commit_message>
Added 2013 to problems-database
</commit_message>
<xml_diff>
--- a/past-competitions/problems-database.xlsx
+++ b/past-competitions/problems-database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gideon Tong\Documents\GitHub\CodeQuest\past-competitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23ABA2C-D00A-42D8-9CE4-0A5B9CEC7993}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3863CABA-F70C-4170-917D-D8D49BC1A294}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1420" windowWidth="20520" windowHeight="12930" xr2:uid="{9AFF80B1-2FDD-49BA-9F8B-87CF455A0979}"/>
+    <workbookView xWindow="1120" yWindow="1420" windowWidth="20520" windowHeight="12940" xr2:uid="{9AFF80B1-2FDD-49BA-9F8B-87CF455A0979}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Year</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>circuits</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>networking</t>
+  </si>
+  <si>
+    <t>encryption</t>
+  </si>
+  <si>
+    <t>puzzle</t>
+  </si>
+  <si>
+    <t>dictionary</t>
+  </si>
+  <si>
+    <t>array</t>
   </si>
 </sst>
 </file>
@@ -427,9 +445,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009FF990-46F2-4A2C-BECD-5761BFAD10EA}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -482,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D19" si="0">C3/214</f>
+        <f t="shared" ref="D3:D36" si="0">C3/214</f>
         <v>1.4018691588785047E-2</v>
       </c>
       <c r="E3" t="s">
@@ -787,6 +808,330 @@
       </c>
       <c r="F19" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2013</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>C20/117</f>
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D36" si="1">C21/117</f>
+        <v>1.7094017094017096E-2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2013</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2013</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2013</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>3.4188034188034191E-2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2013</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>3.4188034188034191E-2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2013</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>4.2735042735042736E-2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2013</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>5.128205128205128E-2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2013</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>5.128205128205128E-2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2013</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>5.9829059829059832E-2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2013</v>
+      </c>
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>6.8376068376068383E-2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2013</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>6.8376068376068383E-2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>2013</v>
+      </c>
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>8.5470085470085472E-2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2013</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>8.5470085470085472E-2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2013</v>
+      </c>
+      <c r="B34">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>9.4017094017094016E-2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2013</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>0.11965811965811966</v>
+      </c>
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2013</v>
+      </c>
+      <c r="B36">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>0.12820512820512819</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>